<commit_message>
update ERD & Date Subtract
</commit_message>
<xml_diff>
--- a/DataDict.xlsx
+++ b/DataDict.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17301"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASC\Documents\Visual Studio 2013\Projects\MarathonSkills2015-TO6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Doc. Arrival\Visual Studio 2015\Projects\MarathonSkills2015-TO6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -663,7 +663,7 @@
   <dimension ref="B2:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="C112" t="s">
         <v>88</v>

</xml_diff>